<commit_message>
integrate storages and renewables into workflow
</commit_message>
<xml_diff>
--- a/amiris_data_structure.xlsx
+++ b/amiris_data_structure.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\TradeRES\toolbox-amiris-emlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857A95D3-05A1-4BB9-B890-F216CC6AA22D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2E39C5-09F5-4BF3-ADFD-99CF2CC38551}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conventionals" sheetId="1" r:id="rId1"/>
+    <sheet name="storages" sheetId="2" r:id="rId2"/>
+    <sheet name="renewables" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">conventionals!$A$1:$G$273</definedName>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="17">
   <si>
     <t>identifier</t>
   </si>
@@ -57,12 +59,30 @@
   <si>
     <t>Efficiency</t>
   </si>
+  <si>
+    <t>EnergyToPowerRatio</t>
+  </si>
+  <si>
+    <t>ChargingEfficiency</t>
+  </si>
+  <si>
+    <t>DischargingEfficiency</t>
+  </si>
+  <si>
+    <t>InitialEnergyLevelInMWH</t>
+  </si>
+  <si>
+    <t>StorageType</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +95,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -421,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6722,4 +6751,89 @@
   <autoFilter ref="A1:G273" xr:uid="{0E53D378-7D65-4DFE-9A24-68D3230363FF}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C455A06-856F-48C9-BCA3-9CB772578DE9}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>10000000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0.9</v>
+      </c>
+      <c r="F2">
+        <v>0.9</v>
+      </c>
+      <c r="G2">
+        <v>30000</v>
+      </c>
+      <c r="H2">
+        <v>8000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2D0D10-B91B-40EE-BB76-00CD4D0E9084}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>